<commit_message>
Backlog and Sprintlog changes
</commit_message>
<xml_diff>
--- a/Week 1/CST-247-RS-SprintProductLogTemplate.xlsx
+++ b/Week 1/CST-247-RS-SprintProductLogTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\CST-247\Week 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5264B2-23A7-410B-B9C9-2A565A2C2146}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC14FB9F-CC14-4458-BDA8-0D532F6D31A9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Project Title:</t>
   </si>
@@ -58,6 +58,24 @@
   </si>
   <si>
     <t>Modification Date</t>
+  </si>
+  <si>
+    <t>Create Backlog</t>
+  </si>
+  <si>
+    <t>Team Meeting</t>
+  </si>
+  <si>
+    <t>Team is on the same page</t>
+  </si>
+  <si>
+    <t>Team understands what to do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentation </t>
+  </si>
+  <si>
+    <t>Everything is recorded</t>
   </si>
 </sst>
 </file>
@@ -225,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -273,6 +291,8 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,7 +576,7 @@
   <dimension ref="A1:I2060"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +586,7 @@
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="20.140625" customWidth="1"/>
     <col min="9" max="9" width="21.42578125" customWidth="1"/>
@@ -632,33 +652,63 @@
       <c r="B4" s="8"/>
       <c r="C4" s="15"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="7"/>
+      <c r="E4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="14">
+        <v>1</v>
+      </c>
+      <c r="H4" s="21">
+        <v>43345</v>
+      </c>
+      <c r="I4" s="22">
+        <v>43345</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="15"/>
       <c r="D5" s="10"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="7"/>
+      <c r="E5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="14">
+        <v>1</v>
+      </c>
+      <c r="H5" s="21">
+        <v>43345</v>
+      </c>
+      <c r="I5" s="22">
+        <v>43345</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="15"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="7"/>
+      <c r="E6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="14">
+        <v>1</v>
+      </c>
+      <c r="H6" s="21">
+        <v>43345</v>
+      </c>
+      <c r="I6" s="22">
+        <v>43345</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
@@ -23268,6 +23318,83 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <DocumentBusinessValueTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Normal</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">581d4866-74cc-43f1-bef1-bb304cbfeaa5</TermId>
+        </TermInfo>
+      </Terms>
+    </DocumentBusinessValueTaxHTField0>
+    <DocumentComments xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <DocumentDepartmentTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Academic Program and Course Development</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">59abafec-cbf5-4238-a796-a3b74278f4db</TermId>
+        </TermInfo>
+      </Terms>
+    </DocumentDepartmentTaxHTField0>
+    <DocumentCategoryTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </DocumentCategoryTaxHTField0>
+    <DocumentTypeTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </DocumentTypeTaxHTField0>
+    <TaxKeywordTaxHTField xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <CourseVersion xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd" xsi:nil="true"/>
+    <SecurityClassificationTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">98311b30-b9e9-4d4f-9f64-0688c0d4a234</TermId>
+        </TermInfo>
+      </Terms>
+    </SecurityClassificationTaxHTField0>
+    <TaxCatchAll xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd">
+      <Value>3</Value>
+      <Value>2</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <DocumentSubjectTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </DocumentSubjectTaxHTField0>
+    <DocumentStatusTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </DocumentStatusTaxHTField0>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>False</openByDefault>
+  <xsnScope/>
+</customXsn>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Course Development" ma:contentTypeID="0x010100A30BC5E90BED914E81F4B67CDEADBEEF0072B4D5296E9CCD41A4B955E8BC4A98B900B6D41DF35BCF664B888FA24C3105B583" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new Course Development document." ma:contentTypeScope="" ma:versionID="9dd9ed6e3bbe7b4f5b00c4ab3cb49488">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="30a82cfc-8d0b-455e-b705-4035c60ff9fd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f302115a5f8a1b15560b600ae7cd187" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -23496,84 +23623,48 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A856C235-C1E3-486A-AF6F-91B1EB05F3BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="30a82cfc-8d0b-455e-b705-4035c60ff9fd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>False</openByDefault>
-  <xsnScope/>
-</customXsn>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C5499EA-2107-4096-9690-EDC799091AC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1713361C-F80E-4293-9FB3-5DC100B81DE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <DocumentBusinessValueTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Normal</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">581d4866-74cc-43f1-bef1-bb304cbfeaa5</TermId>
-        </TermInfo>
-      </Terms>
-    </DocumentBusinessValueTaxHTField0>
-    <DocumentComments xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <DocumentDepartmentTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Academic Program and Course Development</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">59abafec-cbf5-4238-a796-a3b74278f4db</TermId>
-        </TermInfo>
-      </Terms>
-    </DocumentDepartmentTaxHTField0>
-    <DocumentCategoryTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </DocumentCategoryTaxHTField0>
-    <DocumentTypeTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </DocumentTypeTaxHTField0>
-    <TaxKeywordTaxHTField xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <CourseVersion xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd" xsi:nil="true"/>
-    <SecurityClassificationTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">98311b30-b9e9-4d4f-9f64-0688c0d4a234</TermId>
-        </TermInfo>
-      </Terms>
-    </SecurityClassificationTaxHTField0>
-    <TaxCatchAll xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd">
-      <Value>3</Value>
-      <Value>2</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <DocumentSubjectTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </DocumentSubjectTaxHTField0>
-    <DocumentStatusTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </DocumentStatusTaxHTField0>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{543DFEB0-7AA3-434C-B1C2-BCF78AB39365}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68741204-811B-4110-9B64-9D55504528C5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23590,45 +23681,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{543DFEB0-7AA3-434C-B1C2-BCF78AB39365}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1713361C-F80E-4293-9FB3-5DC100B81DE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C5499EA-2107-4096-9690-EDC799091AC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A856C235-C1E3-486A-AF6F-91B1EB05F3BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="30a82cfc-8d0b-455e-b705-4035c60ff9fd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>